<commit_message>
add index_stock_cons_sina for get hs300
</commit_message>
<xml_diff>
--- a/roic2019.xlsx
+++ b/roic2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\ROIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\Roic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -880,7 +880,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +898,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -924,9 +933,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1233,11 +1243,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="A2:O55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
@@ -1285,2540 +1298,2540 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
         <v>92.329101815395191</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <v>59.721819286088952</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>35.888283459426248</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <v>19.493441994597362</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>38.367848246704192</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="2">
         <v>92.329101815395191</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>238.5921504535211</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>105.05075896714889</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>26.163426471010538</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>26.81488469014851</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <v>19.765671330982311</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="2">
         <v>13.86738244637265</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <v>29.449855264130221</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="2">
         <v>21.027636347161732</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <v>52.676356709435993</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>63.236530817033412</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>73.805821986240758</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>36.22327835231372</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>18.88453805780042</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <v>20.69818133606422</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>21.89124246678988</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>19.059792758529159</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>20.54973885379442</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>42.971212798784961</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>49.482933386397882</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>45.405982217876392</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>28.361520310741639</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>15.09153223014609</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <v>16.296402138157891</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>19.284982163395</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>22.415298277119931</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>19.332227526224269</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <v>29.619678252921371</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>45.050475289011501</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>19.878467942775082</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>27.928426346842059</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>27.099555216761889</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <v>13.124951784722571</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
         <v>15.46765049620098</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>15.513152010652361</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>14.701918097191969</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="2">
         <v>24.968816502126341</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>-0.35834069219393339</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>-6.1276666880987589</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1.03069361612365</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>-6.1790472773528604</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.76525366338438694</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>-17.822628010506431</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>1.248031389436195</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>26.047977475063391</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <v>35.499641358386029</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <v>37.577610481786728</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="2">
         <v>29.958597902373629</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <v>9.8216957152260118</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>25.785968033128789</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="2">
         <v>20.93188340762854</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>14.04816057184374</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>10.618592744617731</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>13.53414199186126</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>28.832852964667619</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>13.799023778011041</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>3.410248591205109</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>12.59937877167294</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>20.578139300442949</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <v>29.20330033640457</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <v>14.261532169919819</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="2">
         <v>8.0757683039851713</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="2">
         <v>22.394372275228768</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <v>14.910557583044589</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="2">
         <v>20.79360613617348</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
         <v>20.768905957052809</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
         <v>18.98944637215163</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="2">
         <v>20.08432724172545</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="2">
         <v>9.3645224765811204</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="2">
         <v>16.146098696819401</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="2">
         <v>20.768905957052809</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>20.03108656959343</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>25.702048529225241</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>23.674614556122179</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>18.556048760976669</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>21.40235867107323</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="2">
         <v>20.777863275795479</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="2">
         <v>21.11579272771792</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="2">
         <v>20.91982644784003</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="2">
         <v>20.455362589329361</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="2">
         <v>20.830327254962441</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="2">
         <v>20.24542356928179</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>18.02953875292291</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>18.876471344842209</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>19.222989701632031</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>8.157491549205945</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>18.444472929182819</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>20.38461012554378</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>18.996977127156271</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>19.282369420350019</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>21.280432186362809</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <v>19.77405052600578</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="2">
         <v>22.962884655828962</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="2">
         <v>20.128442058721841</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
         <v>20.95512574685219</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="2">
         <v>19.853259577956361</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
         <v>31.719961039197479</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>15.778249411391069</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>16.872080705572561</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>19.535443599792249</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>21.252120243044448</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>21.59963645757497</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>18.899024950191979</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="2">
         <v>17.414339969520309</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="2">
         <v>18.698320761668381</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="2">
         <v>17.26005443857073</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="2">
         <v>15.691939807319731</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="2">
         <v>17.216771669186279</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="2">
         <v>19.304333792429091</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>39.835470848545583</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>6.7493922979959446</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>5.5936269557816356</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>2.7720274903079041</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>-0.26281140361440952</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>-0.58380538556619732</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>1.90972283715576</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>25.53278511144774</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>28.397097939041519</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <v>15.78291409316606</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>13.617953727307279</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="2">
         <v>15.14664904497161</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="2">
         <v>14.84917228848165</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="2">
         <v>18.613201962548342</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
         <v>19.976540675844809</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>16.805651561689789</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="2">
         <v>16.832213617185399</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="2">
         <v>13.464899274795069</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="2">
         <v>13.848461849736969</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="2">
         <v>11.94734269841163</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="2">
         <v>13.08690127431456</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="2">
         <v>17.871468618240002</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>19.529360882911341</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>22.840576617192479</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>19.11065190828721</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>19.22472924562372</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>19.26065971886344</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>17.547850703644048</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>16.423167078616821</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>18.05408508528534</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="2">
         <v>17.224255238972511</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="2">
         <v>18.051145270907011</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="2">
         <v>17.608791120333439</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="2">
         <v>18.843572296917241</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="2">
         <v>18.167836229385902</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="2">
         <v>17.233835800958222</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
         <v>38.953233178277799</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>24.085521703300081</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>15.416691930217549</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>17.067297623600219</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <v>17.919376348070251</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="2">
         <v>14.84732129286005</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="2">
         <v>15.79987698804522</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="2">
         <v>10.347610970078209</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="2">
         <v>13.66493641699449</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="2">
         <v>16.801121967296009</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
         <v>21.603503164313711</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="2">
         <v>10.0470082094223</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="2">
         <v>6.0772980378135939</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="2">
         <v>3.664307904353818</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="2">
         <v>5.6062416314759496</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="2">
         <v>5.1159491912144546</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="2">
         <v>15.82525568686801</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
         <v>9.5063148430633699</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>7.7887989123659009</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>8.5035193472926291</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>9.9831967002246724</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>12.20676540161767</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>14.46441780226872</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>15.159074451323351</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <v>17.585963025314879</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="2">
         <v>17.27483340944816</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="2">
         <v>14.621431653580609</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="2">
         <v>14.371515879796091</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="2">
         <v>15.42259364760829</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <v>15.73648509296898</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
         <v>35.696257731731173</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>18.672830604462099</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>13.73820043140579</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="2">
         <v>13.88788318271085</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="2">
         <v>14.2276140082219</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="2">
         <v>14.08853456627036</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="2">
         <v>14.11322913582336</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="2">
         <v>14.143125903438539</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="2">
         <v>15.432971406192911</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>37.979259859241211</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>18.99568152685681</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>19.57235128613862</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>21.077312108117269</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>25.4935940518309</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>17.030299379128511</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>14.8529054827055</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="2">
         <v>15.26519552396169</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <v>14.93652163044627</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="2">
         <v>15.222299869850961</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="2">
         <v>16.242078694531092</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="2">
         <v>13.67068263024974</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="2">
         <v>15.0450203982106</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="2">
         <v>15.01820754570449</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>16.066579477180131</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>37.380816018133743</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>26.755732282547509</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>13.618956905818781</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>9.917726517882457</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>12.298219755607519</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <v>13.76542057066457</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <v>13.292217561152709</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <v>16.247898057396469</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="2">
         <v>15.25617504995871</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="2">
         <v>18.636778216708631</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="2">
         <v>18.233312981327149</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="2">
         <v>17.37542208266483</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="2">
         <v>14.43517872973792</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>14.877729127445891</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>14.226354225240421</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>17.393089865597808</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>17.01338226130305</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>16.114588046751411</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>15.429903818128819</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>15.10449708591841</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>14.686669104810271</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <v>12.48316547572794</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="2">
         <v>12.507915112480831</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <v>13.041767498637199</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="2">
         <v>10.789910847082419</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="2">
         <v>12.113197819400151</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="2">
         <v>14.091443888818869</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>9.4225716351675146</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>9.6415113190738264</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>11.94514912761068</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>13.107590870890951</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>14.85233870967742</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>18.08345992904222</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <v>15.375197811679611</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="2">
         <v>14.352322079322381</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>12.28544329024753</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="2">
         <v>11.5696182654995</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="2">
         <v>11.367132360686821</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="2">
         <v>8.2771082202263475</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="2">
         <v>10.404619615470891</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="2">
         <v>14.00432106041651</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>22.286759919256461</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>20.935060042034969</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>11.231416616581109</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>10.13844585401926</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>14.19756811519837</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>15.9508058801083</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <v>17.079944600154072</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <v>16.165926299014949</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>8.5802680740696751</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2">
         <v>7.9297277343201511</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="2">
         <v>8.7239263932614026</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="2">
         <v>7.9513978587994369</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="2">
         <v>8.2016839954603302</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="2">
         <v>13.9420463244129</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
         <v>25.151529061457548</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>31.857723761811791</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>15.82762317181812</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>13.14661225221375</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <v>12.66669327543266</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <v>13.386131316831509</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="2">
         <v>12.49125870087471</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="2">
         <v>11.7976066668726</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="2">
         <v>12.55833222819294</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="2">
         <v>13.880309566488179</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
         <v>13.393469771677159</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>4.2470883190069584</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>1.096298128653403</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>-0.13394532288607081</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>1.4640050010540859</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>19.639303875362021</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>18.965986138905329</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <v>20.360559991441178</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>13.91806221235481</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="2">
         <v>23.675358047568821</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="2">
         <v>19.317993417121599</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="2">
         <v>13.356431671773811</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>6.5427288087082571</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>8.9474865104559509</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>16.27067024873778</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>17.43586231544699</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>18.11899809770383</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>15.642269222835541</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="2">
         <v>14.00654101562254</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="2">
         <v>14.422593742716</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="2">
         <v>11.23562847478714</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
         <v>13.276963884694039</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="2">
         <v>17.983143354167741</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="2">
         <v>19.99451086547861</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="2">
         <v>17.084872701446791</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="2">
         <v>13.221587744375229</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>14.623481363199859</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>6.6763789342474293</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>7.318308811220029</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>9.333794080750824</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>9.3066664248479132</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>10.209158784995561</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <v>12.11595338825218</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="2">
         <v>13.278971206431191</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="2">
         <v>14.08073872398197</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="2">
         <v>8.9706898977002698</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="2">
         <v>11.54003290888353</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="2">
         <v>12.666868437203121</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="2">
         <v>11.05919708126231</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="2">
         <v>13.158554439555109</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
         <v>18.006490583678371</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="2">
         <v>7.9947637047911506</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="2">
         <v>8.3474340791226584</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="2">
         <v>7.3327055642304906</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="2">
         <v>4.6023988343441999</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="2">
         <v>6.7608461592324502</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="2">
         <v>13.000627144234761</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <v>37.94933839966847</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>8.4314040794116814</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>11.19396340482524</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>8.7944487231659707</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>13.236469556006989</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>13.29194077010847</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="2">
         <v>13.26828845827216</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="2">
         <v>12.186359446542269</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="2">
         <v>11.77518259954549</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="2">
         <v>11.57792320947974</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="2">
         <v>7.1409458551659277</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="2">
         <v>10.16468388806372</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="2">
         <v>12.915529558307631</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
         <v>11.92547569370698</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>13.98081031694559</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="2">
         <v>14.39438842530028</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="2">
         <v>10.332001308846991</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="2">
         <v>15.61451918701653</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="2">
         <v>12.85624799864379</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="2">
         <v>14.617239819726819</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="2">
         <v>14.362669001795711</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="2">
         <v>12.902400017030949</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>11.00485135853882</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>10.571385703568749</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>11.513284957166229</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>12.48819975047128</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>10.30745809183005</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>10.96578805640814</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>11.240605096741611</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="2">
         <v>13.026507177421641</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="2">
         <v>14.164546357362941</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="2">
         <v>14.258162310503639</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="2">
         <v>15.641906481585981</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="2">
         <v>15.80287221471978</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="2">
         <v>15.234313668936471</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="2">
         <v>12.8105528771754</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>5.6546215880893298</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>9.6571082208652257</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>7.5355735062045159</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>8.3381602405600113</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>17.568088645771219</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>15.161407881225401</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>13.982716727755509</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="2">
         <v>13.71228672519984</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="2">
         <v>10.610567871144131</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="2">
         <v>12.49150275320209</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="2">
         <v>15.20235736557226</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="2">
         <v>18.075247026640358</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="2">
         <v>15.256369048471569</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="2">
         <v>12.768523774699821</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>-14.61954501082297</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>5.2285999954379907</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>5.0451781308788402</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>8.9479445043779329</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>9.0090348920536556</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <v>9.6361223819401776</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <v>10.94190047677766</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="2">
         <v>12.494241881355499</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="2">
         <v>14.49971015452482</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="2">
         <v>12.40617723182773</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="2">
         <v>13.426252883027839</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="2">
         <v>11.50939877243791</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="2">
         <v>12.447276295764491</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="2">
         <v>12.645284170886001</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
         <v>19.724952915104598</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="2">
         <v>13.656705341788239</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="2">
         <v>12.138335985426091</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="2">
         <v>11.895862027666331</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="2">
         <v>12.250412903922481</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="2">
         <v>13.10608955884322</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="2">
         <v>13.996797948779109</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="2">
         <v>13.117766803848269</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="2">
         <v>12.56363445162688</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>8.01027576663245</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>8.4325812702681322</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>6.2502764366743868</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>6.863778606922402</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>9.1786252916737805</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <v>12.33719975568529</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <v>12.437026620140751</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="2">
         <v>12.423957028694661</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="2">
         <v>12.11175909355223</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="2">
         <v>10.103522591594141</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="2">
         <v>8.6695654828844315</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="2">
         <v>11.102254223602211</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="2">
         <v>9.9584474326935926</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="2">
         <v>12.32424758079588</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
         <v>14.42609017116027</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="2">
         <v>14.056634264537029</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="2">
         <v>13.591110126754799</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="2">
         <v>8.9793674898012092</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="2">
         <v>7.4431601725229273</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="2">
         <v>9.155430660554341</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="2">
         <v>8.484523340878523</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="2">
         <v>8.3610380579852634</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="2">
         <v>12.20903729369768</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>10.937445145832591</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>9.403599503516757</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>14.16531033590423</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>16.098629847207469</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>20.141933755809539</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <v>18.401885020705031</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <v>14.049247994673321</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="2">
         <v>11.22334593819272</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="2">
         <v>11.247025978758851</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="2">
         <v>11.925947453535519</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="2">
         <v>9.3789970626854799</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="2">
         <v>10.454335252294969</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="2">
         <v>10.58642658950532</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="2">
         <v>12.173206637208301</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <v>11.896466497596871</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>10.52580602325644</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>13.19432268249024</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <v>15.48961330524971</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="2">
         <v>12.89718853767118</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="2">
         <v>11.402673597494671</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="2">
         <v>11.429133217490779</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="2">
         <v>4.6875907984839031</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="2">
         <v>4.252025939177102</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="2">
         <v>3.6957107236330198</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="2">
         <v>4.2117758204313418</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="2">
         <v>11.90966511755221</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>9.5498315235317328</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>13.96460427461321</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>10.745505942729849</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>10.11571376500968</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>11.575091799172011</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <v>11.32581212264169</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <v>12.176902922106761</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="2">
         <v>11.894562589776831</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="2">
         <v>11.27184153731219</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="2">
         <v>12.10787760131606</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="2">
         <v>12.91357936037133</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="2">
         <v>13.640855152814011</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="2">
         <v>12.88743737150047</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="2">
         <v>11.781102349731929</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
         <v>31.36795252313328</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>8.4793003401946425</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>12.021797574240701</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>12.351083476976109</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>16.51289136736564</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>18.150183483646568</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="2">
         <v>7.5923013647168549</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="2">
         <v>9.4766526611579813</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="2">
         <v>10.64327339395477</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="2">
         <v>8.3365169691834282</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="2">
         <v>4.785308691619699</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="2">
         <v>7.9216996849192993</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="2">
         <v>11.7397125031738</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>11.629353552430469</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>10.458548817312071</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>12.85581517837176</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>15.16074029875052</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>10.588612727692921</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>11.296621783474089</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>11.029993493819131</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
         <v>11.431293568819241</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="2">
         <v>12.450804749415431</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="2">
         <v>10.12005950438817</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="2">
         <v>7.2095681947879022</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="2">
         <v>5.9322601346277253</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="2">
         <v>7.7539626112679327</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="2">
         <v>11.637363937351269</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
         <v>18.007280759600899</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>25.602540591013209</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>11.744399512759159</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>4.4496904813924694</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="2">
         <v>10.234848667073219</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="2">
         <v>19.287589028171951</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="2">
         <v>11.135884980411401</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="2">
         <v>3.573321403798015</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="2">
         <v>12.978707271785289</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="2">
         <v>9.2293045519982382</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="2">
         <v>11.32404272554588</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
         <v>23.081774787121009</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>17.223841111728159</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="2">
         <v>8.071070472099672</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="2">
         <v>8.1671241056369759</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="2">
         <v>7.5386244117863113</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="2">
         <v>6.8197200164441654</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="2">
         <v>-16.703833042007538</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="2">
         <v>-0.78182953792568843</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="2">
         <v>11.154011896488271</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>9.7058483792630135</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>8.0128374938174627</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>8.0716213109771626</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>10.444970810914761</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>12.91616826814867</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="2">
         <v>10.6859899393584</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>10.994674439486291</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="2">
         <v>10.86889386128292</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="2">
         <v>11.53260699803907</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="2">
         <v>13.336792119318559</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="2">
         <v>14.63150137443477</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="2">
         <v>17.6796208855129</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="2">
         <v>15.21597145975541</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="2">
         <v>11.132058432936089</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2">
         <v>40.489212719658838</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="2">
         <v>7.6076534396584909</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>8.8052415246992854</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>-0.74672320219594868</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>-8.3766406650530048</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="2">
         <v>6.368099765875102</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="2">
         <v>10.83291046922508</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="2">
         <v>16.129751517450678</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="2">
         <v>18.103138635080931</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="2">
         <v>14.34776987807734</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="2">
         <v>13.042180248813519</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="2">
         <v>15.16436292065727</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="2">
         <v>11.11025391751696</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>7.1568320779176684</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>8.9244785323158133</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>9.4110598226470277</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>10.063677660908819</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>11.51875442621872</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>13.456959646422201</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="2">
         <v>12.307576686657789</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="2">
         <v>9.8961585957484335</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="2">
         <v>10.80648463688124</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="2">
         <v>15.20212529561099</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="2">
         <v>14.054682264909539</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="2">
         <v>2.2504924616560129</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="2">
         <v>10.502433340725521</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="2">
         <v>11.00340663976249</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <v>12.37178803236419</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>16.101117074597941</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="2">
         <v>15.239119744712021</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>16.03485901944952</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>21.097503513998529</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="2">
         <v>16.984874063834852</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="2">
         <v>11.63663435246257</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="2">
         <v>10.80634903114569</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="2">
         <v>10.11816117244396</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="2">
         <v>12.965534258473321</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="2">
         <v>15.045816041247789</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="2">
         <v>15.787616192185871</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="2">
         <v>14.599655497302329</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="2">
         <v>10.85371485201741</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>13.807456050217651</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>10.61507543556448</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="2">
         <v>13.89418867455057</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>16.641297779024399</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>16.363018150683391</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>13.584740848467</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2">
         <v>11.68702666564374</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
         <v>10.94404821796731</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="2">
         <v>9.845264419927668</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="2">
         <v>13.74310515767632</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="2">
         <v>16.80188982480594</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="2">
         <v>15.23114700140736</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="2">
         <v>15.25871399462987</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="2">
         <v>10.8254464345129</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="2">
         <v>24.921096747338531</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>28.26854287954081</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>28.509681956874111</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>24.464207754945019</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>28.929861298401079</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>24.615692099342521</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>6.7202736356181854</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="2">
         <v>11.32188564449199</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="2">
         <v>13.828532250987269</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="2">
         <v>12.62982010346329</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="2">
         <v>14.578272852346171</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="2">
         <v>15.342863070539419</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="2">
         <v>14.183652008782961</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="2">
         <v>10.62356384369915</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <v>9.8841015544007611</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>7.8207723982470334</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>6.5171455459373062</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>5.8394854813173813</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>4.9530676491849919</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2">
         <v>8.8464262751256939</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <v>13.20172771731105</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="2">
         <v>11.654511522415859</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="2">
         <v>6.7990955619434903</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="2">
         <v>6.5981904005799006</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="2">
         <v>8.7899008547139488</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="2">
         <v>10.859516244409591</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="2">
         <v>8.7492024999011466</v>
       </c>
-      <c r="O51">
+      <c r="O51" s="2">
         <v>10.551778267223471</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="2">
         <v>10.94457286665609</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="2">
         <v>10.26396405280223</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>11.47124198669942</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>13.61677080599698</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>12.317270988564371</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="2">
         <v>12.850680582944539</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <v>13.794299095303479</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="2">
         <v>11.23888990737588</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="2">
         <v>6.1648251176275277</v>
       </c>
-      <c r="K52">
+      <c r="K52" s="2">
         <v>10.835962940628249</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="2">
         <v>11.252317231928741</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="2">
         <v>10.34345127124368</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="2">
         <v>10.810577147933561</v>
       </c>
-      <c r="O52">
+      <c r="O52" s="2">
         <v>10.3993380401023</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <v>0.43907130493629543</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="2">
         <v>4.4195768529793966</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="2">
         <v>6.4080213025833652</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>2.030036597950843</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>3.131012671951706</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="2">
         <v>6.6344577970081344</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="2">
         <v>10.88296306075417</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="2">
         <v>10.928650994251459</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="2">
         <v>9.3617585203267293</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="2">
         <v>6.2977300353356886</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="2">
         <v>0.31693281234456711</v>
       </c>
-      <c r="M53">
+      <c r="M53" s="2">
         <v>-2.909305849077672</v>
       </c>
-      <c r="N53">
+      <c r="N53" s="2">
         <v>1.2351189995341949</v>
       </c>
-      <c r="O53">
+      <c r="O53" s="2">
         <v>10.39112419177745</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="2">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2">
         <v>18.912552785483332</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="2">
         <v>6.294604344361777</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>6.8733297824771826</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="2">
         <v>7.6048398945864584</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="2">
         <v>8.5002314935384362</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="2">
         <v>9.1673220815386411</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="2">
         <v>9.2548625095355259</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="2">
         <v>12.28823470334358</v>
       </c>
-      <c r="K54">
+      <c r="K54" s="2">
         <v>12.34563570570255</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="2">
         <v>11.80040463336168</v>
       </c>
-      <c r="M54">
+      <c r="M54" s="2">
         <v>12.201285198032799</v>
       </c>
-      <c r="N54">
+      <c r="N54" s="2">
         <v>12.115775179032349</v>
       </c>
-      <c r="O54">
+      <c r="O54" s="2">
         <v>10.23680643147258</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <v>12.80791034540839</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>15.22147507867628</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="2">
         <v>19.179990669937201</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>19.059099779105129</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>18.561356712477149</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="2">
         <v>9.9734755420118724</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>5.5880178603032586</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="2">
         <v>12.698056420906889</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="2">
         <v>12.347533571255751</v>
       </c>
-      <c r="K55">
+      <c r="K55" s="2">
         <v>6.0006205293523527</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="2">
         <v>-13.050916371747469</v>
       </c>
-      <c r="M55">
+      <c r="M55" s="2">
         <v>4.9096067695370831</v>
       </c>
-      <c r="N55">
+      <c r="N55" s="2">
         <v>-0.71356302428601237</v>
       </c>
-      <c r="O55">
+      <c r="O55" s="2">
         <v>10.211202617488629</v>
       </c>
     </row>

</xml_diff>